<commit_message>
added additional turn parameters to xls
</commit_message>
<xml_diff>
--- a/dummy data.xlsx
+++ b/dummy data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>Training Type</t>
   </si>
@@ -149,6 +149,33 @@
   </si>
   <si>
     <t>Do I feel weel rested?</t>
+  </si>
+  <si>
+    <t>Average G Force</t>
+  </si>
+  <si>
+    <t>Maximum G Force</t>
+  </si>
+  <si>
+    <t>Average Slope</t>
+  </si>
+  <si>
+    <t>Maximum Slope</t>
+  </si>
+  <si>
+    <t>G Force at Maximum Slope</t>
+  </si>
+  <si>
+    <t>Turn Radius</t>
+  </si>
+  <si>
+    <t>Turn Type</t>
+  </si>
+  <si>
+    <t>Carving</t>
+  </si>
+  <si>
+    <t>Skidding</t>
   </si>
 </sst>
 </file>
@@ -501,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A11C08-C4F8-4CBE-9A19-BA4B29C05FF9}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -519,7 +546,7 @@
     <col min="10" max="10" width="13.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -550,8 +577,29 @@
       <c r="J1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B2" s="1">
         <v>42461</v>
       </c>
@@ -567,8 +615,11 @@
       <c r="F2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="Q2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
         <v>1</v>
       </c>
@@ -581,8 +632,11 @@
       <c r="F3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="Q3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>1</v>
       </c>
@@ -596,7 +650,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>1</v>
       </c>
@@ -607,7 +661,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -618,7 +672,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="C7" t="s">
         <v>2</v>
       </c>
@@ -626,7 +680,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="C8" t="s">
         <v>2</v>
       </c>
@@ -634,7 +688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="C9" t="s">
         <v>2</v>
       </c>
@@ -642,7 +696,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
         <v>2</v>
       </c>
@@ -650,7 +704,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="C11" t="s">
         <v>2</v>
       </c>

</xml_diff>